<commit_message>
added Jordan to the Excel master file
</commit_message>
<xml_diff>
--- a/lit review data/Jordan peer-reviewed list 04192021 HA .xlsx
+++ b/lit review data/Jordan peer-reviewed list 04192021 HA .xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamad\Desktop\MECP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamad\Desktop\My-Github\localrepo\lit review data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8001BDA8-884C-4988-AD80-960682537B6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB24555-5DBA-4232-9FCD-0DFA603BEF52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{173FAFC4-260D-4237-AF51-AA6388A28C3E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1716" uniqueCount="1266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="1263">
   <si>
     <t>Delaying surgery for patients with a previous SARS-CoV-2 infection</t>
   </si>
@@ -1778,12 +1778,6 @@
     <t>BACKGROUND: Intensive care and ventilator capacities are essential for treatment of COVID-19 patients. Severely injured patients are often in continuous need of intensive care and ventilator treatment. The question arises, whether restrictions related to COVID-19 have led to a decrease in severely injured patients and thus to an increase in intensive care unit (ICU) capacity. MATERIAL AND METHODS: A retrospective analysis of all seriously injured patients with an injury severity score (ISS) ≥16 was performed between 17 March and 30 April 2020 at a level 1 trauma center in Germany. The mechanism of injury and the ISS were recorded. Further data were collected as to whether it was a work-related accident, a documented suicide attempt and if surgery was necessary in the first 24 h after arrival in hospital. Data from 2018 and 2019 served as a control group. RESULTS: There was no substantial difference in the total number of seriously injured patients (2018 n = 30, 2019 n = 23, 2020 n = 27). Furthermore, there was no relevant difference in the number of patients needing intensive care or ventilator treatment when leaving the shock room. The number of patients needing an operative intervention within the first 24 h after arriving at hospital was slightly higher in 2020. The mean ISS was at a constant level during all 3 years. In 2020 there was no polytraumatized motorbike rider, who did not have a work-related accident (2018 n = 5, 2019 n = 4, 2020 n = 0). A noticeable increase in work-related accidents was observed (2018: 10%, 2019: 26.1%, 2020 44.4%). DISCUSSION: Restrictions related to COVID-19 did not lead to a reduction in seriously injured patients needing ICU care. Due to the monocentric data analysis there is room for misinterpretation. In general, intensive care and operating capacities should be managed with adequate consideration for seriously injured patients even in times of crisis, such as the COVID-19 pandemic. Confirmation through the German Trauma Register is pending.</t>
   </si>
   <si>
-    <t>Publisher: Abstract available from the publisher.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ger </t>
-  </si>
-  <si>
     <t>M. D. Galbraith, K. T. Kinning, K. D. Sullivan, R. Baxter, P. Araya, K. R. Jordan, S. Russell, K. P. Smith, R. E. Granrath, J. Shaw, M. Dzieciatkowska, T. Ghosh, A. A. Monte, A. D'Alessandro, K. C. Hansen, T. D. Bennett, E. W. Y. Hsieh and J. M. Espinosa</t>
   </si>
   <si>
@@ -1815,9 +1809,6 @@
   </si>
   <si>
     <t>OBJECTIVE: Controversial results on remdesivir efficacy have been reported. We aimed to report our real-life experience with the use of remdesivir from its availability in Spain. METHODS: We performed a descriptive study of all patients admitted for ≥48 hours with confirmed COVID-19 who received remdesivir between the 1st of July and the 30th of September 2020. RESULTS: A total of 123 patients out of 242 admitted with COVID-19 at our hospital (50.8%) received remdesivir. Median age was 58 years, 61% were males and 56.9 % received at least one anti-inflammatory treatment. No adverse events requiring remdesivir discontinuation were reported. The need of intensive care unit admission, mechanical ventilation and 30-days mortality were 19.5%, 7.3% and 4.1%, respectively. CONCLUSIONS: In our real-life experience, the use of remdesivir in hospitalized patients with COVID-19 was associated with a low mortality rate and good safety profile.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spa </t>
   </si>
   <si>
     <t>M. J. Gelfand, J. C. Jackson, X. Pan, D. Nau, D. Pieper, E. Denison, M. Dagher, P. A. M. Van Lange, C. Y. Chiu and M. Wang</t>
@@ -3886,8 +3877,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{817CC852-F6EA-4F03-AE23-747B2C307937}" name="Table1" displayName="Table1" ref="A1:D444" totalsRowShown="0">
-  <autoFilter ref="A1:D444" xr:uid="{E8919D7D-DA1E-4C76-8BC7-6400D61B2DE7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{817CC852-F6EA-4F03-AE23-747B2C307937}" name="Table1" displayName="Table1" ref="A1:D440" totalsRowShown="0">
+  <autoFilter ref="A1:D440" xr:uid="{E8919D7D-DA1E-4C76-8BC7-6400D61B2DE7}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{806728B3-0423-46D5-B826-3679D154DE92}" name="Author"/>
     <tableColumn id="2" xr3:uid="{B7E95031-F7A1-4029-8B9E-8B2FFE3CAB70}" name="Year"/>
@@ -4195,10 +4186,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{514736EC-A8EB-4525-AF8A-8F05FCAF18E5}">
-  <dimension ref="A1:E444"/>
+  <dimension ref="A1:E440"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A440" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D440"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4208,16 +4199,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D1" t="s">
         <v>1262</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1263</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1264</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1265</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -7603,27 +7594,48 @@
       <c r="A205" t="s">
         <v>581</v>
       </c>
+      <c r="B205">
+        <v>2020</v>
+      </c>
+      <c r="C205" t="s">
+        <v>582</v>
+      </c>
+      <c r="D205" t="s">
+        <v>583</v>
+      </c>
+      <c r="E205" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
+        <v>584</v>
+      </c>
+      <c r="B206">
+        <v>2021</v>
+      </c>
+      <c r="C206" t="s">
         <v>582</v>
       </c>
-      <c r="B206" t="s">
+      <c r="D206" t="s">
+        <v>585</v>
+      </c>
+      <c r="E206" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="B207">
         <v>2020</v>
       </c>
       <c r="C207" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="D207" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="E207" t="s">
         <v>1</v>
@@ -7631,33 +7643,30 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="B208">
         <v>2021</v>
       </c>
       <c r="C208" t="s">
-        <v>584</v>
+        <v>590</v>
       </c>
       <c r="D208" t="s">
-        <v>587</v>
-      </c>
-      <c r="E208" t="s">
-        <v>1</v>
+        <v>591</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
       <c r="B209">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C209" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
       <c r="D209" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
       <c r="E209" t="s">
         <v>1</v>
@@ -7665,43 +7674,67 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="B210">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C210" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
       <c r="D210" t="s">
-        <v>593</v>
+        <v>597</v>
+      </c>
+      <c r="E210" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>581</v>
+        <v>598</v>
+      </c>
+      <c r="B211">
+        <v>2020</v>
+      </c>
+      <c r="C211" t="s">
+        <v>599</v>
+      </c>
+      <c r="D211" t="s">
+        <v>600</v>
+      </c>
+      <c r="E211" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>594</v>
-      </c>
-      <c r="B212" t="s">
+        <v>601</v>
+      </c>
+      <c r="B212">
+        <v>2021</v>
+      </c>
+      <c r="C212" t="s">
+        <v>602</v>
+      </c>
+      <c r="D212" t="s">
+        <v>603</v>
+      </c>
+      <c r="E212" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>595</v>
+        <v>604</v>
       </c>
       <c r="B213">
         <v>2021</v>
       </c>
       <c r="C213" t="s">
-        <v>596</v>
+        <v>605</v>
       </c>
       <c r="D213" t="s">
-        <v>597</v>
+        <v>606</v>
       </c>
       <c r="E213" t="s">
         <v>1</v>
@@ -7709,16 +7742,16 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>598</v>
+        <v>607</v>
       </c>
       <c r="B214">
         <v>2020</v>
       </c>
       <c r="C214" t="s">
-        <v>599</v>
+        <v>608</v>
       </c>
       <c r="D214" t="s">
-        <v>600</v>
+        <v>609</v>
       </c>
       <c r="E214" t="s">
         <v>1</v>
@@ -7726,16 +7759,13 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>601</v>
+        <v>610</v>
       </c>
       <c r="B215">
         <v>2020</v>
       </c>
       <c r="C215" t="s">
-        <v>602</v>
-      </c>
-      <c r="D215" t="s">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="E215" t="s">
         <v>1</v>
@@ -7743,16 +7773,13 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>604</v>
+        <v>612</v>
       </c>
       <c r="B216">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C216" t="s">
-        <v>605</v>
-      </c>
-      <c r="D216" t="s">
-        <v>606</v>
+        <v>613</v>
       </c>
       <c r="E216" t="s">
         <v>1</v>
@@ -7760,16 +7787,16 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>607</v>
+        <v>614</v>
       </c>
       <c r="B217">
         <v>2021</v>
       </c>
       <c r="C217" t="s">
-        <v>608</v>
+        <v>615</v>
       </c>
       <c r="D217" t="s">
-        <v>609</v>
+        <v>616</v>
       </c>
       <c r="E217" t="s">
         <v>1</v>
@@ -7777,16 +7804,16 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>610</v>
+        <v>617</v>
       </c>
       <c r="B218">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C218" t="s">
-        <v>611</v>
+        <v>618</v>
       </c>
       <c r="D218" t="s">
-        <v>612</v>
+        <v>619</v>
       </c>
       <c r="E218" t="s">
         <v>1</v>
@@ -7794,13 +7821,16 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>613</v>
+        <v>620</v>
       </c>
       <c r="B219">
         <v>2020</v>
       </c>
       <c r="C219" t="s">
-        <v>614</v>
+        <v>621</v>
+      </c>
+      <c r="D219" t="s">
+        <v>622</v>
       </c>
       <c r="E219" t="s">
         <v>1</v>
@@ -7808,13 +7838,16 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>615</v>
+        <v>623</v>
       </c>
       <c r="B220">
         <v>2020</v>
       </c>
       <c r="C220" t="s">
-        <v>616</v>
+        <v>624</v>
+      </c>
+      <c r="D220" t="s">
+        <v>625</v>
       </c>
       <c r="E220" t="s">
         <v>1</v>
@@ -7822,16 +7855,16 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>617</v>
+        <v>626</v>
       </c>
       <c r="B221">
         <v>2021</v>
       </c>
       <c r="C221" t="s">
-        <v>618</v>
+        <v>627</v>
       </c>
       <c r="D221" t="s">
-        <v>619</v>
+        <v>628</v>
       </c>
       <c r="E221" t="s">
         <v>1</v>
@@ -7839,16 +7872,16 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>620</v>
+        <v>629</v>
       </c>
       <c r="B222">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C222" t="s">
-        <v>621</v>
+        <v>630</v>
       </c>
       <c r="D222" t="s">
-        <v>622</v>
+        <v>631</v>
       </c>
       <c r="E222" t="s">
         <v>1</v>
@@ -7856,16 +7889,16 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>623</v>
+        <v>632</v>
       </c>
       <c r="B223">
         <v>2020</v>
       </c>
       <c r="C223" t="s">
-        <v>624</v>
+        <v>633</v>
       </c>
       <c r="D223" t="s">
-        <v>625</v>
+        <v>634</v>
       </c>
       <c r="E223" t="s">
         <v>1</v>
@@ -7873,16 +7906,16 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>626</v>
+        <v>635</v>
       </c>
       <c r="B224">
         <v>2020</v>
       </c>
       <c r="C224" t="s">
-        <v>627</v>
+        <v>636</v>
       </c>
       <c r="D224" t="s">
-        <v>628</v>
+        <v>637</v>
       </c>
       <c r="E224" t="s">
         <v>1</v>
@@ -7890,16 +7923,16 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>629</v>
+        <v>638</v>
       </c>
       <c r="B225">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C225" t="s">
-        <v>630</v>
+        <v>639</v>
       </c>
       <c r="D225" t="s">
-        <v>631</v>
+        <v>640</v>
       </c>
       <c r="E225" t="s">
         <v>1</v>
@@ -7907,16 +7940,16 @@
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>632</v>
+        <v>641</v>
       </c>
       <c r="B226">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C226" t="s">
-        <v>633</v>
+        <v>642</v>
       </c>
       <c r="D226" t="s">
-        <v>634</v>
+        <v>643</v>
       </c>
       <c r="E226" t="s">
         <v>1</v>
@@ -7924,16 +7957,16 @@
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
       <c r="B227">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C227" t="s">
-        <v>636</v>
+        <v>645</v>
       </c>
       <c r="D227" t="s">
-        <v>637</v>
+        <v>646</v>
       </c>
       <c r="E227" t="s">
         <v>1</v>
@@ -7941,16 +7974,16 @@
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B228">
         <v>2020</v>
       </c>
       <c r="C228" t="s">
-        <v>639</v>
+        <v>648</v>
       </c>
       <c r="D228" t="s">
-        <v>640</v>
+        <v>649</v>
       </c>
       <c r="E228" t="s">
         <v>1</v>
@@ -7958,16 +7991,16 @@
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>641</v>
+        <v>650</v>
       </c>
       <c r="B229">
         <v>2020</v>
       </c>
       <c r="C229" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="D229" t="s">
-        <v>643</v>
+        <v>652</v>
       </c>
       <c r="E229" t="s">
         <v>1</v>
@@ -7975,16 +8008,16 @@
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>644</v>
+        <v>653</v>
       </c>
       <c r="B230">
         <v>2021</v>
       </c>
       <c r="C230" t="s">
-        <v>645</v>
+        <v>654</v>
       </c>
       <c r="D230" t="s">
-        <v>646</v>
+        <v>655</v>
       </c>
       <c r="E230" t="s">
         <v>1</v>
@@ -7992,16 +8025,16 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>647</v>
+        <v>656</v>
       </c>
       <c r="B231">
         <v>2021</v>
       </c>
       <c r="C231" t="s">
-        <v>648</v>
+        <v>657</v>
       </c>
       <c r="D231" t="s">
-        <v>649</v>
+        <v>658</v>
       </c>
       <c r="E231" t="s">
         <v>1</v>
@@ -8009,16 +8042,16 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>650</v>
+        <v>659</v>
       </c>
       <c r="B232">
         <v>2020</v>
       </c>
       <c r="C232" t="s">
-        <v>651</v>
+        <v>660</v>
       </c>
       <c r="D232" t="s">
-        <v>652</v>
+        <v>661</v>
       </c>
       <c r="E232" t="s">
         <v>1</v>
@@ -8026,16 +8059,16 @@
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>653</v>
+        <v>662</v>
       </c>
       <c r="B233">
         <v>2020</v>
       </c>
       <c r="C233" t="s">
-        <v>654</v>
+        <v>663</v>
       </c>
       <c r="D233" t="s">
-        <v>655</v>
+        <v>664</v>
       </c>
       <c r="E233" t="s">
         <v>1</v>
@@ -8043,16 +8076,16 @@
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>656</v>
+        <v>665</v>
       </c>
       <c r="B234">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C234" t="s">
-        <v>657</v>
+        <v>666</v>
       </c>
       <c r="D234" t="s">
-        <v>658</v>
+        <v>667</v>
       </c>
       <c r="E234" t="s">
         <v>1</v>
@@ -8060,16 +8093,16 @@
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>659</v>
+        <v>668</v>
       </c>
       <c r="B235">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C235" t="s">
-        <v>660</v>
+        <v>669</v>
       </c>
       <c r="D235" t="s">
-        <v>661</v>
+        <v>670</v>
       </c>
       <c r="E235" t="s">
         <v>1</v>
@@ -8077,16 +8110,16 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>662</v>
+        <v>671</v>
       </c>
       <c r="B236">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C236" t="s">
-        <v>663</v>
+        <v>672</v>
       </c>
       <c r="D236" t="s">
-        <v>664</v>
+        <v>673</v>
       </c>
       <c r="E236" t="s">
         <v>1</v>
@@ -8094,16 +8127,16 @@
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>665</v>
+        <v>674</v>
       </c>
       <c r="B237">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C237" t="s">
-        <v>666</v>
+        <v>675</v>
       </c>
       <c r="D237" t="s">
-        <v>667</v>
+        <v>676</v>
       </c>
       <c r="E237" t="s">
         <v>1</v>
@@ -8111,16 +8144,13 @@
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>668</v>
+        <v>677</v>
       </c>
       <c r="B238">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C238" t="s">
-        <v>669</v>
-      </c>
-      <c r="D238" t="s">
-        <v>670</v>
+        <v>678</v>
       </c>
       <c r="E238" t="s">
         <v>1</v>
@@ -8128,16 +8158,13 @@
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>671</v>
+        <v>677</v>
       </c>
       <c r="B239">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C239" t="s">
-        <v>672</v>
-      </c>
-      <c r="D239" t="s">
-        <v>673</v>
+        <v>679</v>
       </c>
       <c r="E239" t="s">
         <v>1</v>
@@ -8145,16 +8172,16 @@
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>674</v>
+        <v>680</v>
       </c>
       <c r="B240">
         <v>2021</v>
       </c>
       <c r="C240" t="s">
-        <v>675</v>
+        <v>681</v>
       </c>
       <c r="D240" t="s">
-        <v>676</v>
+        <v>682</v>
       </c>
       <c r="E240" t="s">
         <v>1</v>
@@ -8162,16 +8189,16 @@
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>677</v>
+        <v>683</v>
       </c>
       <c r="B241">
-        <v>2021</v>
+        <v>2013</v>
       </c>
       <c r="C241" t="s">
-        <v>678</v>
+        <v>684</v>
       </c>
       <c r="D241" t="s">
-        <v>679</v>
+        <v>685</v>
       </c>
       <c r="E241" t="s">
         <v>1</v>
@@ -8179,13 +8206,16 @@
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>680</v>
+        <v>686</v>
       </c>
       <c r="B242">
         <v>2021</v>
       </c>
       <c r="C242" t="s">
-        <v>681</v>
+        <v>687</v>
+      </c>
+      <c r="D242" t="s">
+        <v>688</v>
       </c>
       <c r="E242" t="s">
         <v>1</v>
@@ -8193,13 +8223,16 @@
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>680</v>
+        <v>689</v>
       </c>
       <c r="B243">
         <v>2021</v>
       </c>
       <c r="C243" t="s">
-        <v>682</v>
+        <v>690</v>
+      </c>
+      <c r="D243" t="s">
+        <v>691</v>
       </c>
       <c r="E243" t="s">
         <v>1</v>
@@ -8207,16 +8240,16 @@
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>683</v>
+        <v>692</v>
       </c>
       <c r="B244">
         <v>2021</v>
       </c>
       <c r="C244" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="D244" t="s">
-        <v>685</v>
+        <v>694</v>
       </c>
       <c r="E244" t="s">
         <v>1</v>
@@ -8224,16 +8257,16 @@
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>686</v>
+        <v>695</v>
       </c>
       <c r="B245">
-        <v>2013</v>
+        <v>2021</v>
       </c>
       <c r="C245" t="s">
-        <v>687</v>
+        <v>696</v>
       </c>
       <c r="D245" t="s">
-        <v>688</v>
+        <v>697</v>
       </c>
       <c r="E245" t="s">
         <v>1</v>
@@ -8241,16 +8274,16 @@
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>689</v>
+        <v>698</v>
       </c>
       <c r="B246">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C246" t="s">
-        <v>690</v>
+        <v>699</v>
       </c>
       <c r="D246" t="s">
-        <v>691</v>
+        <v>700</v>
       </c>
       <c r="E246" t="s">
         <v>1</v>
@@ -8258,16 +8291,16 @@
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>692</v>
+        <v>701</v>
       </c>
       <c r="B247">
         <v>2021</v>
       </c>
       <c r="C247" t="s">
-        <v>693</v>
+        <v>702</v>
       </c>
       <c r="D247" t="s">
-        <v>694</v>
+        <v>703</v>
       </c>
       <c r="E247" t="s">
         <v>1</v>
@@ -8275,16 +8308,16 @@
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>695</v>
+        <v>704</v>
       </c>
       <c r="B248">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C248" t="s">
-        <v>696</v>
+        <v>705</v>
       </c>
       <c r="D248" t="s">
-        <v>697</v>
+        <v>706</v>
       </c>
       <c r="E248" t="s">
         <v>1</v>
@@ -8292,16 +8325,16 @@
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>698</v>
+        <v>707</v>
       </c>
       <c r="B249">
         <v>2021</v>
       </c>
       <c r="C249" t="s">
-        <v>699</v>
+        <v>708</v>
       </c>
       <c r="D249" t="s">
-        <v>700</v>
+        <v>709</v>
       </c>
       <c r="E249" t="s">
         <v>1</v>
@@ -8309,16 +8342,16 @@
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>701</v>
+        <v>710</v>
       </c>
       <c r="B250">
         <v>2020</v>
       </c>
       <c r="C250" t="s">
-        <v>702</v>
+        <v>711</v>
       </c>
       <c r="D250" t="s">
-        <v>703</v>
+        <v>712</v>
       </c>
       <c r="E250" t="s">
         <v>1</v>
@@ -8326,16 +8359,16 @@
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="B251">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C251" t="s">
-        <v>705</v>
+        <v>714</v>
       </c>
       <c r="D251" t="s">
-        <v>706</v>
+        <v>715</v>
       </c>
       <c r="E251" t="s">
         <v>1</v>
@@ -8343,16 +8376,16 @@
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>707</v>
+        <v>716</v>
       </c>
       <c r="B252">
         <v>2020</v>
       </c>
       <c r="C252" t="s">
-        <v>708</v>
+        <v>717</v>
       </c>
       <c r="D252" t="s">
-        <v>709</v>
+        <v>718</v>
       </c>
       <c r="E252" t="s">
         <v>1</v>
@@ -8360,16 +8393,16 @@
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>710</v>
+        <v>719</v>
       </c>
       <c r="B253">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C253" t="s">
-        <v>711</v>
+        <v>720</v>
       </c>
       <c r="D253" t="s">
-        <v>712</v>
+        <v>721</v>
       </c>
       <c r="E253" t="s">
         <v>1</v>
@@ -8377,16 +8410,16 @@
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="B254">
         <v>2020</v>
       </c>
       <c r="C254" t="s">
-        <v>714</v>
+        <v>723</v>
       </c>
       <c r="D254" t="s">
-        <v>715</v>
+        <v>724</v>
       </c>
       <c r="E254" t="s">
         <v>1</v>
@@ -8394,16 +8427,16 @@
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>716</v>
+        <v>725</v>
       </c>
       <c r="B255">
         <v>2020</v>
       </c>
       <c r="C255" t="s">
-        <v>717</v>
+        <v>726</v>
       </c>
       <c r="D255" t="s">
-        <v>718</v>
+        <v>727</v>
       </c>
       <c r="E255" t="s">
         <v>1</v>
@@ -8411,16 +8444,16 @@
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>719</v>
+        <v>728</v>
       </c>
       <c r="B256">
         <v>2020</v>
       </c>
       <c r="C256" t="s">
-        <v>720</v>
+        <v>729</v>
       </c>
       <c r="D256" t="s">
-        <v>721</v>
+        <v>730</v>
       </c>
       <c r="E256" t="s">
         <v>1</v>
@@ -8428,16 +8461,16 @@
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>722</v>
+        <v>731</v>
       </c>
       <c r="B257">
         <v>2020</v>
       </c>
       <c r="C257" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
       <c r="D257" t="s">
-        <v>724</v>
+        <v>733</v>
       </c>
       <c r="E257" t="s">
         <v>1</v>
@@ -8445,16 +8478,16 @@
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>725</v>
+        <v>734</v>
       </c>
       <c r="B258">
         <v>2020</v>
       </c>
       <c r="C258" t="s">
-        <v>726</v>
+        <v>735</v>
       </c>
       <c r="D258" t="s">
-        <v>727</v>
+        <v>736</v>
       </c>
       <c r="E258" t="s">
         <v>1</v>
@@ -8462,16 +8495,16 @@
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>728</v>
+        <v>737</v>
       </c>
       <c r="B259">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C259" t="s">
-        <v>729</v>
+        <v>738</v>
       </c>
       <c r="D259" t="s">
-        <v>730</v>
+        <v>739</v>
       </c>
       <c r="E259" t="s">
         <v>1</v>
@@ -8479,16 +8512,16 @@
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>731</v>
+        <v>740</v>
       </c>
       <c r="B260">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C260" t="s">
-        <v>732</v>
+        <v>741</v>
       </c>
       <c r="D260" t="s">
-        <v>733</v>
+        <v>742</v>
       </c>
       <c r="E260" t="s">
         <v>1</v>
@@ -8496,16 +8529,16 @@
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>734</v>
+        <v>743</v>
       </c>
       <c r="B261">
         <v>2020</v>
       </c>
       <c r="C261" t="s">
-        <v>735</v>
+        <v>744</v>
       </c>
       <c r="D261" t="s">
-        <v>736</v>
+        <v>745</v>
       </c>
       <c r="E261" t="s">
         <v>1</v>
@@ -8513,16 +8546,16 @@
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>737</v>
+        <v>746</v>
       </c>
       <c r="B262">
         <v>2020</v>
       </c>
       <c r="C262" t="s">
-        <v>738</v>
+        <v>747</v>
       </c>
       <c r="D262" t="s">
-        <v>739</v>
+        <v>748</v>
       </c>
       <c r="E262" t="s">
         <v>1</v>
@@ -8530,16 +8563,13 @@
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>740</v>
+        <v>749</v>
       </c>
       <c r="B263">
         <v>2021</v>
       </c>
       <c r="C263" t="s">
-        <v>741</v>
-      </c>
-      <c r="D263" t="s">
-        <v>742</v>
+        <v>750</v>
       </c>
       <c r="E263" t="s">
         <v>1</v>
@@ -8547,16 +8577,16 @@
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>743</v>
+        <v>751</v>
       </c>
       <c r="B264">
         <v>2021</v>
       </c>
       <c r="C264" t="s">
-        <v>744</v>
+        <v>752</v>
       </c>
       <c r="D264" t="s">
-        <v>745</v>
+        <v>753</v>
       </c>
       <c r="E264" t="s">
         <v>1</v>
@@ -8564,16 +8594,16 @@
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>746</v>
+        <v>754</v>
       </c>
       <c r="B265">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C265" t="s">
-        <v>747</v>
+        <v>755</v>
       </c>
       <c r="D265" t="s">
-        <v>748</v>
+        <v>756</v>
       </c>
       <c r="E265" t="s">
         <v>1</v>
@@ -8581,16 +8611,13 @@
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>749</v>
+        <v>757</v>
       </c>
       <c r="B266">
         <v>2020</v>
       </c>
       <c r="C266" t="s">
-        <v>750</v>
-      </c>
-      <c r="D266" t="s">
-        <v>751</v>
+        <v>758</v>
       </c>
       <c r="E266" t="s">
         <v>1</v>
@@ -8598,13 +8625,13 @@
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
-        <v>752</v>
+        <v>759</v>
       </c>
       <c r="B267">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C267" t="s">
-        <v>753</v>
+        <v>760</v>
       </c>
       <c r="E267" t="s">
         <v>1</v>
@@ -8612,16 +8639,16 @@
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>754</v>
+        <v>761</v>
       </c>
       <c r="B268">
         <v>2021</v>
       </c>
       <c r="C268" t="s">
-        <v>755</v>
+        <v>762</v>
       </c>
       <c r="D268" t="s">
-        <v>756</v>
+        <v>763</v>
       </c>
       <c r="E268" t="s">
         <v>1</v>
@@ -8629,16 +8656,13 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>757</v>
+        <v>764</v>
       </c>
       <c r="B269">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C269" t="s">
-        <v>758</v>
-      </c>
-      <c r="D269" t="s">
-        <v>759</v>
+        <v>765</v>
       </c>
       <c r="E269" t="s">
         <v>1</v>
@@ -8646,13 +8670,16 @@
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>760</v>
+        <v>766</v>
       </c>
       <c r="B270">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C270" t="s">
-        <v>761</v>
+        <v>767</v>
+      </c>
+      <c r="D270" t="s">
+        <v>768</v>
       </c>
       <c r="E270" t="s">
         <v>1</v>
@@ -8660,13 +8687,16 @@
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>762</v>
+        <v>769</v>
       </c>
       <c r="B271">
         <v>2020</v>
       </c>
       <c r="C271" t="s">
-        <v>763</v>
+        <v>770</v>
+      </c>
+      <c r="D271" t="s">
+        <v>771</v>
       </c>
       <c r="E271" t="s">
         <v>1</v>
@@ -8674,16 +8704,13 @@
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>764</v>
+        <v>772</v>
       </c>
       <c r="B272">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C272" t="s">
-        <v>765</v>
-      </c>
-      <c r="D272" t="s">
-        <v>766</v>
+        <v>773</v>
       </c>
       <c r="E272" t="s">
         <v>1</v>
@@ -8691,13 +8718,13 @@
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
-        <v>767</v>
+        <v>772</v>
       </c>
       <c r="B273">
         <v>2020</v>
       </c>
       <c r="C273" t="s">
-        <v>768</v>
+        <v>774</v>
       </c>
       <c r="E273" t="s">
         <v>1</v>
@@ -8705,16 +8732,13 @@
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
-        <v>769</v>
+        <v>775</v>
       </c>
       <c r="B274">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C274" t="s">
-        <v>770</v>
-      </c>
-      <c r="D274" t="s">
-        <v>771</v>
+        <v>776</v>
       </c>
       <c r="E274" t="s">
         <v>1</v>
@@ -8722,16 +8746,16 @@
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
-        <v>772</v>
+        <v>777</v>
       </c>
       <c r="B275">
         <v>2020</v>
       </c>
       <c r="C275" t="s">
-        <v>773</v>
+        <v>778</v>
       </c>
       <c r="D275" t="s">
-        <v>774</v>
+        <v>779</v>
       </c>
       <c r="E275" t="s">
         <v>1</v>
@@ -8739,13 +8763,16 @@
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
-        <v>775</v>
+        <v>780</v>
       </c>
       <c r="B276">
         <v>2020</v>
       </c>
       <c r="C276" t="s">
-        <v>776</v>
+        <v>781</v>
+      </c>
+      <c r="D276" t="s">
+        <v>782</v>
       </c>
       <c r="E276" t="s">
         <v>1</v>
@@ -8753,13 +8780,16 @@
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
-        <v>775</v>
+        <v>783</v>
       </c>
       <c r="B277">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C277" t="s">
-        <v>777</v>
+        <v>784</v>
+      </c>
+      <c r="D277" t="s">
+        <v>785</v>
       </c>
       <c r="E277" t="s">
         <v>1</v>
@@ -8767,13 +8797,16 @@
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
-        <v>778</v>
+        <v>786</v>
       </c>
       <c r="B278">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C278" t="s">
-        <v>779</v>
+        <v>787</v>
+      </c>
+      <c r="D278" t="s">
+        <v>788</v>
       </c>
       <c r="E278" t="s">
         <v>1</v>
@@ -8781,16 +8814,16 @@
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
-        <v>780</v>
+        <v>789</v>
       </c>
       <c r="B279">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C279" t="s">
-        <v>781</v>
+        <v>790</v>
       </c>
       <c r="D279" t="s">
-        <v>782</v>
+        <v>791</v>
       </c>
       <c r="E279" t="s">
         <v>1</v>
@@ -8798,16 +8831,16 @@
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
-        <v>783</v>
+        <v>792</v>
       </c>
       <c r="B280">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C280" t="s">
-        <v>784</v>
+        <v>793</v>
       </c>
       <c r="D280" t="s">
-        <v>785</v>
+        <v>794</v>
       </c>
       <c r="E280" t="s">
         <v>1</v>
@@ -8815,16 +8848,16 @@
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
-        <v>786</v>
+        <v>795</v>
       </c>
       <c r="B281">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C281" t="s">
-        <v>787</v>
+        <v>796</v>
       </c>
       <c r="D281" t="s">
-        <v>788</v>
+        <v>797</v>
       </c>
       <c r="E281" t="s">
         <v>1</v>
@@ -8832,16 +8865,16 @@
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
-        <v>789</v>
+        <v>798</v>
       </c>
       <c r="B282">
         <v>2021</v>
       </c>
       <c r="C282" t="s">
-        <v>790</v>
+        <v>799</v>
       </c>
       <c r="D282" t="s">
-        <v>791</v>
+        <v>800</v>
       </c>
       <c r="E282" t="s">
         <v>1</v>
@@ -8849,16 +8882,16 @@
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
-        <v>792</v>
+        <v>801</v>
       </c>
       <c r="B283">
         <v>2021</v>
       </c>
       <c r="C283" t="s">
-        <v>793</v>
+        <v>802</v>
       </c>
       <c r="D283" t="s">
-        <v>794</v>
+        <v>803</v>
       </c>
       <c r="E283" t="s">
         <v>1</v>
@@ -8866,16 +8899,16 @@
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
-        <v>795</v>
+        <v>804</v>
       </c>
       <c r="B284">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C284" t="s">
-        <v>796</v>
+        <v>805</v>
       </c>
       <c r="D284" t="s">
-        <v>797</v>
+        <v>806</v>
       </c>
       <c r="E284" t="s">
         <v>1</v>
@@ -8883,16 +8916,16 @@
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
-        <v>798</v>
+        <v>807</v>
       </c>
       <c r="B285">
         <v>2020</v>
       </c>
       <c r="C285" t="s">
-        <v>799</v>
+        <v>808</v>
       </c>
       <c r="D285" t="s">
-        <v>800</v>
+        <v>809</v>
       </c>
       <c r="E285" t="s">
         <v>1</v>
@@ -8900,16 +8933,13 @@
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>801</v>
+        <v>810</v>
       </c>
       <c r="B286">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C286" t="s">
-        <v>802</v>
-      </c>
-      <c r="D286" t="s">
-        <v>803</v>
+        <v>811</v>
       </c>
       <c r="E286" t="s">
         <v>1</v>
@@ -8917,16 +8947,16 @@
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>804</v>
+        <v>812</v>
       </c>
       <c r="B287">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C287" t="s">
-        <v>805</v>
+        <v>813</v>
       </c>
       <c r="D287" t="s">
-        <v>806</v>
+        <v>814</v>
       </c>
       <c r="E287" t="s">
         <v>1</v>
@@ -8934,16 +8964,16 @@
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
-        <v>807</v>
+        <v>815</v>
       </c>
       <c r="B288">
         <v>2020</v>
       </c>
       <c r="C288" t="s">
-        <v>808</v>
+        <v>816</v>
       </c>
       <c r="D288" t="s">
-        <v>809</v>
+        <v>817</v>
       </c>
       <c r="E288" t="s">
         <v>1</v>
@@ -8951,16 +8981,16 @@
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
-        <v>810</v>
+        <v>818</v>
       </c>
       <c r="B289">
         <v>2020</v>
       </c>
       <c r="C289" t="s">
-        <v>811</v>
+        <v>819</v>
       </c>
       <c r="D289" t="s">
-        <v>812</v>
+        <v>820</v>
       </c>
       <c r="E289" t="s">
         <v>1</v>
@@ -8968,13 +8998,16 @@
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
-        <v>813</v>
+        <v>821</v>
       </c>
       <c r="B290">
         <v>2020</v>
       </c>
       <c r="C290" t="s">
-        <v>814</v>
+        <v>822</v>
+      </c>
+      <c r="D290" t="s">
+        <v>823</v>
       </c>
       <c r="E290" t="s">
         <v>1</v>
@@ -8982,16 +9015,16 @@
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
-        <v>815</v>
+        <v>824</v>
       </c>
       <c r="B291">
         <v>2020</v>
       </c>
       <c r="C291" t="s">
-        <v>816</v>
+        <v>825</v>
       </c>
       <c r="D291" t="s">
-        <v>817</v>
+        <v>826</v>
       </c>
       <c r="E291" t="s">
         <v>1</v>
@@ -8999,16 +9032,16 @@
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
-        <v>818</v>
+        <v>827</v>
       </c>
       <c r="B292">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C292" t="s">
-        <v>819</v>
+        <v>828</v>
       </c>
       <c r="D292" t="s">
-        <v>820</v>
+        <v>829</v>
       </c>
       <c r="E292" t="s">
         <v>1</v>
@@ -9016,16 +9049,16 @@
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
-        <v>821</v>
+        <v>830</v>
       </c>
       <c r="B293">
         <v>2020</v>
       </c>
       <c r="C293" t="s">
-        <v>822</v>
+        <v>831</v>
       </c>
       <c r="D293" t="s">
-        <v>823</v>
+        <v>832</v>
       </c>
       <c r="E293" t="s">
         <v>1</v>
@@ -9033,16 +9066,16 @@
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
-        <v>824</v>
+        <v>833</v>
       </c>
       <c r="B294">
         <v>2020</v>
       </c>
       <c r="C294" t="s">
-        <v>825</v>
+        <v>834</v>
       </c>
       <c r="D294" t="s">
-        <v>826</v>
+        <v>835</v>
       </c>
       <c r="E294" t="s">
         <v>1</v>
@@ -9050,16 +9083,16 @@
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
-        <v>827</v>
+        <v>836</v>
       </c>
       <c r="B295">
         <v>2020</v>
       </c>
       <c r="C295" t="s">
-        <v>828</v>
+        <v>837</v>
       </c>
       <c r="D295" t="s">
-        <v>829</v>
+        <v>838</v>
       </c>
       <c r="E295" t="s">
         <v>1</v>
@@ -9067,16 +9100,16 @@
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
-        <v>830</v>
+        <v>839</v>
       </c>
       <c r="B296">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C296" t="s">
-        <v>831</v>
+        <v>840</v>
       </c>
       <c r="D296" t="s">
-        <v>832</v>
+        <v>841</v>
       </c>
       <c r="E296" t="s">
         <v>1</v>
@@ -9084,16 +9117,16 @@
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
-        <v>833</v>
+        <v>842</v>
       </c>
       <c r="B297">
         <v>2020</v>
       </c>
       <c r="C297" t="s">
-        <v>834</v>
+        <v>843</v>
       </c>
       <c r="D297" t="s">
-        <v>835</v>
+        <v>844</v>
       </c>
       <c r="E297" t="s">
         <v>1</v>
@@ -9101,16 +9134,16 @@
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
-        <v>836</v>
+        <v>842</v>
       </c>
       <c r="B298">
         <v>2020</v>
       </c>
       <c r="C298" t="s">
-        <v>837</v>
+        <v>845</v>
       </c>
       <c r="D298" t="s">
-        <v>838</v>
+        <v>846</v>
       </c>
       <c r="E298" t="s">
         <v>1</v>
@@ -9118,16 +9151,16 @@
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
-        <v>839</v>
+        <v>847</v>
       </c>
       <c r="B299">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C299" t="s">
-        <v>840</v>
+        <v>848</v>
       </c>
       <c r="D299" t="s">
-        <v>841</v>
+        <v>849</v>
       </c>
       <c r="E299" t="s">
         <v>1</v>
@@ -9135,16 +9168,16 @@
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
-        <v>842</v>
+        <v>850</v>
       </c>
       <c r="B300">
         <v>2020</v>
       </c>
       <c r="C300" t="s">
-        <v>843</v>
+        <v>851</v>
       </c>
       <c r="D300" t="s">
-        <v>844</v>
+        <v>852</v>
       </c>
       <c r="E300" t="s">
         <v>1</v>
@@ -9152,16 +9185,16 @@
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
-        <v>845</v>
+        <v>853</v>
       </c>
       <c r="B301">
         <v>2020</v>
       </c>
       <c r="C301" t="s">
-        <v>846</v>
+        <v>854</v>
       </c>
       <c r="D301" t="s">
-        <v>847</v>
+        <v>855</v>
       </c>
       <c r="E301" t="s">
         <v>1</v>
@@ -9169,16 +9202,16 @@
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
-        <v>845</v>
+        <v>853</v>
       </c>
       <c r="B302">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C302" t="s">
-        <v>848</v>
+        <v>856</v>
       </c>
       <c r="D302" t="s">
-        <v>849</v>
+        <v>857</v>
       </c>
       <c r="E302" t="s">
         <v>1</v>
@@ -9186,16 +9219,16 @@
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
-        <v>850</v>
+        <v>858</v>
       </c>
       <c r="B303">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C303" t="s">
-        <v>851</v>
+        <v>859</v>
       </c>
       <c r="D303" t="s">
-        <v>852</v>
+        <v>860</v>
       </c>
       <c r="E303" t="s">
         <v>1</v>
@@ -9203,16 +9236,16 @@
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
-        <v>853</v>
+        <v>861</v>
       </c>
       <c r="B304">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C304" t="s">
-        <v>854</v>
+        <v>862</v>
       </c>
       <c r="D304" t="s">
-        <v>855</v>
+        <v>863</v>
       </c>
       <c r="E304" t="s">
         <v>1</v>
@@ -9220,16 +9253,16 @@
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="B305">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C305" t="s">
-        <v>857</v>
+        <v>865</v>
       </c>
       <c r="D305" t="s">
-        <v>858</v>
+        <v>866</v>
       </c>
       <c r="E305" t="s">
         <v>1</v>
@@ -9237,16 +9270,16 @@
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
-        <v>856</v>
+        <v>867</v>
       </c>
       <c r="B306">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C306" t="s">
-        <v>859</v>
+        <v>868</v>
       </c>
       <c r="D306" t="s">
-        <v>860</v>
+        <v>869</v>
       </c>
       <c r="E306" t="s">
         <v>1</v>
@@ -9254,16 +9287,16 @@
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
-        <v>861</v>
+        <v>870</v>
       </c>
       <c r="B307">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C307" t="s">
-        <v>862</v>
+        <v>871</v>
       </c>
       <c r="D307" t="s">
-        <v>863</v>
+        <v>872</v>
       </c>
       <c r="E307" t="s">
         <v>1</v>
@@ -9271,16 +9304,16 @@
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
-        <v>864</v>
+        <v>873</v>
       </c>
       <c r="B308">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C308" t="s">
-        <v>865</v>
+        <v>874</v>
       </c>
       <c r="D308" t="s">
-        <v>866</v>
+        <v>875</v>
       </c>
       <c r="E308" t="s">
         <v>1</v>
@@ -9288,16 +9321,16 @@
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
-        <v>867</v>
+        <v>876</v>
       </c>
       <c r="B309">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C309" t="s">
-        <v>868</v>
+        <v>877</v>
       </c>
       <c r="D309" t="s">
-        <v>869</v>
+        <v>878</v>
       </c>
       <c r="E309" t="s">
         <v>1</v>
@@ -9305,16 +9338,16 @@
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
-        <v>870</v>
+        <v>879</v>
       </c>
       <c r="B310">
         <v>2020</v>
       </c>
       <c r="C310" t="s">
-        <v>871</v>
+        <v>880</v>
       </c>
       <c r="D310" t="s">
-        <v>872</v>
+        <v>881</v>
       </c>
       <c r="E310" t="s">
         <v>1</v>
@@ -9322,16 +9355,13 @@
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
-        <v>873</v>
+        <v>882</v>
       </c>
       <c r="B311">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C311" t="s">
-        <v>874</v>
-      </c>
-      <c r="D311" t="s">
-        <v>875</v>
+        <v>883</v>
       </c>
       <c r="E311" t="s">
         <v>1</v>
@@ -9339,16 +9369,16 @@
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
-        <v>876</v>
+        <v>884</v>
       </c>
       <c r="B312">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C312" t="s">
-        <v>877</v>
+        <v>885</v>
       </c>
       <c r="D312" t="s">
-        <v>878</v>
+        <v>886</v>
       </c>
       <c r="E312" t="s">
         <v>1</v>
@@ -9356,16 +9386,16 @@
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
-        <v>879</v>
+        <v>887</v>
       </c>
       <c r="B313">
         <v>2020</v>
       </c>
       <c r="C313" t="s">
-        <v>880</v>
+        <v>888</v>
       </c>
       <c r="D313" t="s">
-        <v>881</v>
+        <v>889</v>
       </c>
       <c r="E313" t="s">
         <v>1</v>
@@ -9373,16 +9403,13 @@
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
-        <v>882</v>
+        <v>890</v>
       </c>
       <c r="B314">
         <v>2020</v>
       </c>
       <c r="C314" t="s">
-        <v>883</v>
-      </c>
-      <c r="D314" t="s">
-        <v>884</v>
+        <v>891</v>
       </c>
       <c r="E314" t="s">
         <v>1</v>
@@ -9390,13 +9417,16 @@
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
-        <v>885</v>
+        <v>892</v>
       </c>
       <c r="B315">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C315" t="s">
-        <v>886</v>
+        <v>893</v>
+      </c>
+      <c r="D315" t="s">
+        <v>894</v>
       </c>
       <c r="E315" t="s">
         <v>1</v>
@@ -9404,16 +9434,16 @@
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
-        <v>887</v>
+        <v>895</v>
       </c>
       <c r="B316">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C316" t="s">
-        <v>888</v>
+        <v>896</v>
       </c>
       <c r="D316" t="s">
-        <v>889</v>
+        <v>897</v>
       </c>
       <c r="E316" t="s">
         <v>1</v>
@@ -9421,16 +9451,16 @@
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
-        <v>890</v>
+        <v>898</v>
       </c>
       <c r="B317">
         <v>2020</v>
       </c>
       <c r="C317" t="s">
-        <v>891</v>
+        <v>899</v>
       </c>
       <c r="D317" t="s">
-        <v>892</v>
+        <v>900</v>
       </c>
       <c r="E317" t="s">
         <v>1</v>
@@ -9438,13 +9468,16 @@
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
-        <v>893</v>
+        <v>901</v>
       </c>
       <c r="B318">
         <v>2020</v>
       </c>
       <c r="C318" t="s">
-        <v>894</v>
+        <v>902</v>
+      </c>
+      <c r="D318" t="s">
+        <v>903</v>
       </c>
       <c r="E318" t="s">
         <v>1</v>
@@ -9452,16 +9485,16 @@
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
-        <v>895</v>
+        <v>904</v>
       </c>
       <c r="B319">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C319" t="s">
-        <v>896</v>
+        <v>905</v>
       </c>
       <c r="D319" t="s">
-        <v>897</v>
+        <v>906</v>
       </c>
       <c r="E319" t="s">
         <v>1</v>
@@ -9469,16 +9502,16 @@
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
-        <v>898</v>
+        <v>907</v>
       </c>
       <c r="B320">
         <v>2020</v>
       </c>
       <c r="C320" t="s">
-        <v>899</v>
+        <v>908</v>
       </c>
       <c r="D320" t="s">
-        <v>900</v>
+        <v>909</v>
       </c>
       <c r="E320" t="s">
         <v>1</v>
@@ -9486,16 +9519,13 @@
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B321">
         <v>2020</v>
       </c>
       <c r="C321" t="s">
-        <v>902</v>
-      </c>
-      <c r="D321" t="s">
-        <v>903</v>
+        <v>911</v>
       </c>
       <c r="E321" t="s">
         <v>1</v>
@@ -9503,16 +9533,16 @@
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
-        <v>904</v>
+        <v>912</v>
       </c>
       <c r="B322">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C322" t="s">
-        <v>905</v>
+        <v>913</v>
       </c>
       <c r="D322" t="s">
-        <v>906</v>
+        <v>914</v>
       </c>
       <c r="E322" t="s">
         <v>1</v>
@@ -9520,16 +9550,16 @@
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
-        <v>907</v>
+        <v>915</v>
       </c>
       <c r="B323">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C323" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="D323" t="s">
-        <v>909</v>
+        <v>917</v>
       </c>
       <c r="E323" t="s">
         <v>1</v>
@@ -9537,16 +9567,16 @@
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
-        <v>910</v>
+        <v>918</v>
       </c>
       <c r="B324">
         <v>2020</v>
       </c>
       <c r="C324" t="s">
-        <v>911</v>
+        <v>919</v>
       </c>
       <c r="D324" t="s">
-        <v>912</v>
+        <v>920</v>
       </c>
       <c r="E324" t="s">
         <v>1</v>
@@ -9554,13 +9584,16 @@
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
-        <v>913</v>
+        <v>921</v>
       </c>
       <c r="B325">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C325" t="s">
-        <v>914</v>
+        <v>922</v>
+      </c>
+      <c r="D325" t="s">
+        <v>923</v>
       </c>
       <c r="E325" t="s">
         <v>1</v>
@@ -9568,16 +9601,16 @@
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
-        <v>915</v>
+        <v>924</v>
       </c>
       <c r="B326">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C326" t="s">
-        <v>916</v>
+        <v>925</v>
       </c>
       <c r="D326" t="s">
-        <v>917</v>
+        <v>926</v>
       </c>
       <c r="E326" t="s">
         <v>1</v>
@@ -9585,16 +9618,16 @@
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
-        <v>918</v>
+        <v>927</v>
       </c>
       <c r="B327">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C327" t="s">
-        <v>919</v>
+        <v>928</v>
       </c>
       <c r="D327" t="s">
-        <v>920</v>
+        <v>929</v>
       </c>
       <c r="E327" t="s">
         <v>1</v>
@@ -9602,16 +9635,16 @@
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
-        <v>921</v>
+        <v>930</v>
       </c>
       <c r="B328">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C328" t="s">
-        <v>922</v>
+        <v>931</v>
       </c>
       <c r="D328" t="s">
-        <v>923</v>
+        <v>932</v>
       </c>
       <c r="E328" t="s">
         <v>1</v>
@@ -9619,16 +9652,16 @@
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
-        <v>924</v>
+        <v>933</v>
       </c>
       <c r="B329">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C329" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="D329" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="E329" t="s">
         <v>1</v>
@@ -9636,16 +9669,16 @@
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="B330">
         <v>2020</v>
       </c>
       <c r="C330" t="s">
-        <v>928</v>
+        <v>937</v>
       </c>
       <c r="D330" t="s">
-        <v>929</v>
+        <v>938</v>
       </c>
       <c r="E330" t="s">
         <v>1</v>
@@ -9653,16 +9686,16 @@
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
-        <v>930</v>
+        <v>939</v>
       </c>
       <c r="B331">
         <v>2020</v>
       </c>
       <c r="C331" t="s">
-        <v>931</v>
+        <v>940</v>
       </c>
       <c r="D331" t="s">
-        <v>932</v>
+        <v>941</v>
       </c>
       <c r="E331" t="s">
         <v>1</v>
@@ -9670,16 +9703,16 @@
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
-        <v>933</v>
+        <v>942</v>
       </c>
       <c r="B332">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C332" t="s">
-        <v>934</v>
+        <v>943</v>
       </c>
       <c r="D332" t="s">
-        <v>935</v>
+        <v>944</v>
       </c>
       <c r="E332" t="s">
         <v>1</v>
@@ -9687,16 +9720,16 @@
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
-        <v>936</v>
+        <v>945</v>
       </c>
       <c r="B333">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C333" t="s">
-        <v>937</v>
+        <v>946</v>
       </c>
       <c r="D333" t="s">
-        <v>938</v>
+        <v>947</v>
       </c>
       <c r="E333" t="s">
         <v>1</v>
@@ -9704,16 +9737,16 @@
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
-        <v>939</v>
+        <v>948</v>
       </c>
       <c r="B334">
         <v>2020</v>
       </c>
       <c r="C334" t="s">
-        <v>940</v>
+        <v>949</v>
       </c>
       <c r="D334" t="s">
-        <v>941</v>
+        <v>950</v>
       </c>
       <c r="E334" t="s">
         <v>1</v>
@@ -9721,16 +9754,13 @@
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
-        <v>942</v>
+        <v>951</v>
       </c>
       <c r="B335">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C335" t="s">
-        <v>943</v>
-      </c>
-      <c r="D335" t="s">
-        <v>944</v>
+        <v>952</v>
       </c>
       <c r="E335" t="s">
         <v>1</v>
@@ -9738,16 +9768,13 @@
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
-        <v>945</v>
+        <v>953</v>
       </c>
       <c r="B336">
         <v>2020</v>
       </c>
       <c r="C336" t="s">
-        <v>946</v>
-      </c>
-      <c r="D336" t="s">
-        <v>947</v>
+        <v>954</v>
       </c>
       <c r="E336" t="s">
         <v>1</v>
@@ -9755,16 +9782,16 @@
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
-        <v>948</v>
+        <v>955</v>
       </c>
       <c r="B337">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C337" t="s">
-        <v>949</v>
+        <v>956</v>
       </c>
       <c r="D337" t="s">
-        <v>950</v>
+        <v>957</v>
       </c>
       <c r="E337" t="s">
         <v>1</v>
@@ -9772,16 +9799,16 @@
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
-        <v>951</v>
+        <v>958</v>
       </c>
       <c r="B338">
         <v>2020</v>
       </c>
       <c r="C338" t="s">
-        <v>952</v>
+        <v>959</v>
       </c>
       <c r="D338" t="s">
-        <v>953</v>
+        <v>960</v>
       </c>
       <c r="E338" t="s">
         <v>1</v>
@@ -9789,13 +9816,16 @@
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
-        <v>954</v>
+        <v>961</v>
       </c>
       <c r="B339">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C339" t="s">
-        <v>955</v>
+        <v>962</v>
+      </c>
+      <c r="D339" t="s">
+        <v>963</v>
       </c>
       <c r="E339" t="s">
         <v>1</v>
@@ -9803,13 +9833,16 @@
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
-        <v>956</v>
+        <v>964</v>
       </c>
       <c r="B340">
         <v>2020</v>
       </c>
       <c r="C340" t="s">
-        <v>957</v>
+        <v>965</v>
+      </c>
+      <c r="D340" t="s">
+        <v>966</v>
       </c>
       <c r="E340" t="s">
         <v>1</v>
@@ -9817,16 +9850,16 @@
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
-        <v>958</v>
+        <v>967</v>
       </c>
       <c r="B341">
         <v>2020</v>
       </c>
       <c r="C341" t="s">
-        <v>959</v>
+        <v>968</v>
       </c>
       <c r="D341" t="s">
-        <v>960</v>
+        <v>969</v>
       </c>
       <c r="E341" t="s">
         <v>1</v>
@@ -9834,16 +9867,16 @@
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
-        <v>961</v>
+        <v>970</v>
       </c>
       <c r="B342">
         <v>2020</v>
       </c>
       <c r="C342" t="s">
-        <v>962</v>
+        <v>971</v>
       </c>
       <c r="D342" t="s">
-        <v>963</v>
+        <v>972</v>
       </c>
       <c r="E342" t="s">
         <v>1</v>
@@ -9851,16 +9884,16 @@
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
-        <v>964</v>
+        <v>973</v>
       </c>
       <c r="B343">
         <v>2020</v>
       </c>
       <c r="C343" t="s">
-        <v>965</v>
+        <v>974</v>
       </c>
       <c r="D343" t="s">
-        <v>966</v>
+        <v>975</v>
       </c>
       <c r="E343" t="s">
         <v>1</v>
@@ -9868,16 +9901,16 @@
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
-        <v>967</v>
+        <v>976</v>
       </c>
       <c r="B344">
         <v>2020</v>
       </c>
       <c r="C344" t="s">
-        <v>968</v>
+        <v>977</v>
       </c>
       <c r="D344" t="s">
-        <v>969</v>
+        <v>978</v>
       </c>
       <c r="E344" t="s">
         <v>1</v>
@@ -9885,16 +9918,16 @@
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
-        <v>970</v>
+        <v>979</v>
       </c>
       <c r="B345">
         <v>2020</v>
       </c>
       <c r="C345" t="s">
-        <v>971</v>
+        <v>980</v>
       </c>
       <c r="D345" t="s">
-        <v>972</v>
+        <v>981</v>
       </c>
       <c r="E345" t="s">
         <v>1</v>
@@ -9902,16 +9935,16 @@
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
-        <v>973</v>
+        <v>982</v>
       </c>
       <c r="B346">
         <v>2020</v>
       </c>
       <c r="C346" t="s">
-        <v>974</v>
+        <v>983</v>
       </c>
       <c r="D346" t="s">
-        <v>975</v>
+        <v>984</v>
       </c>
       <c r="E346" t="s">
         <v>1</v>
@@ -9919,16 +9952,16 @@
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
-        <v>976</v>
+        <v>985</v>
       </c>
       <c r="B347">
         <v>2020</v>
       </c>
       <c r="C347" t="s">
-        <v>977</v>
+        <v>986</v>
       </c>
       <c r="D347" t="s">
-        <v>978</v>
+        <v>987</v>
       </c>
       <c r="E347" t="s">
         <v>1</v>
@@ -9936,16 +9969,16 @@
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
-        <v>979</v>
+        <v>988</v>
       </c>
       <c r="B348">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C348" t="s">
-        <v>980</v>
+        <v>989</v>
       </c>
       <c r="D348" t="s">
-        <v>981</v>
+        <v>990</v>
       </c>
       <c r="E348" t="s">
         <v>1</v>
@@ -9953,16 +9986,16 @@
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
-        <v>982</v>
+        <v>991</v>
       </c>
       <c r="B349">
         <v>2020</v>
       </c>
       <c r="C349" t="s">
-        <v>983</v>
+        <v>992</v>
       </c>
       <c r="D349" t="s">
-        <v>984</v>
+        <v>993</v>
       </c>
       <c r="E349" t="s">
         <v>1</v>
@@ -9970,16 +10003,16 @@
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
-        <v>985</v>
+        <v>994</v>
       </c>
       <c r="B350">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C350" t="s">
-        <v>986</v>
+        <v>995</v>
       </c>
       <c r="D350" t="s">
-        <v>987</v>
+        <v>996</v>
       </c>
       <c r="E350" t="s">
         <v>1</v>
@@ -9987,16 +10020,16 @@
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
-        <v>988</v>
+        <v>997</v>
       </c>
       <c r="B351">
         <v>2020</v>
       </c>
       <c r="C351" t="s">
-        <v>989</v>
+        <v>998</v>
       </c>
       <c r="D351" t="s">
-        <v>990</v>
+        <v>999</v>
       </c>
       <c r="E351" t="s">
         <v>1</v>
@@ -10004,16 +10037,16 @@
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
-        <v>991</v>
+        <v>1000</v>
       </c>
       <c r="B352">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C352" t="s">
-        <v>992</v>
+        <v>1001</v>
       </c>
       <c r="D352" t="s">
-        <v>993</v>
+        <v>1002</v>
       </c>
       <c r="E352" t="s">
         <v>1</v>
@@ -10021,16 +10054,16 @@
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
-        <v>994</v>
+        <v>1003</v>
       </c>
       <c r="B353">
         <v>2020</v>
       </c>
       <c r="C353" t="s">
-        <v>995</v>
+        <v>1004</v>
       </c>
       <c r="D353" t="s">
-        <v>996</v>
+        <v>1005</v>
       </c>
       <c r="E353" t="s">
         <v>1</v>
@@ -10038,16 +10071,16 @@
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
-        <v>997</v>
+        <v>1006</v>
       </c>
       <c r="B354">
         <v>2021</v>
       </c>
       <c r="C354" t="s">
-        <v>998</v>
+        <v>1007</v>
       </c>
       <c r="D354" t="s">
-        <v>999</v>
+        <v>1008</v>
       </c>
       <c r="E354" t="s">
         <v>1</v>
@@ -10055,16 +10088,16 @@
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
-        <v>1000</v>
+        <v>1009</v>
       </c>
       <c r="B355">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C355" t="s">
-        <v>1001</v>
+        <v>1010</v>
       </c>
       <c r="D355" t="s">
-        <v>1002</v>
+        <v>1011</v>
       </c>
       <c r="E355" t="s">
         <v>1</v>
@@ -10072,16 +10105,13 @@
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
-        <v>1003</v>
+        <v>1012</v>
       </c>
       <c r="B356">
         <v>2020</v>
       </c>
       <c r="C356" t="s">
-        <v>1004</v>
-      </c>
-      <c r="D356" t="s">
-        <v>1005</v>
+        <v>1013</v>
       </c>
       <c r="E356" t="s">
         <v>1</v>
@@ -10089,16 +10119,16 @@
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
-        <v>1006</v>
+        <v>1014</v>
       </c>
       <c r="B357">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C357" t="s">
-        <v>1007</v>
+        <v>1015</v>
       </c>
       <c r="D357" t="s">
-        <v>1008</v>
+        <v>1016</v>
       </c>
       <c r="E357" t="s">
         <v>1</v>
@@ -10106,16 +10136,16 @@
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
-        <v>1009</v>
+        <v>1017</v>
       </c>
       <c r="B358">
         <v>2021</v>
       </c>
       <c r="C358" t="s">
-        <v>1010</v>
+        <v>1018</v>
       </c>
       <c r="D358" t="s">
-        <v>1011</v>
+        <v>1019</v>
       </c>
       <c r="E358" t="s">
         <v>1</v>
@@ -10123,16 +10153,16 @@
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
-        <v>1012</v>
+        <v>1020</v>
       </c>
       <c r="B359">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C359" t="s">
-        <v>1013</v>
+        <v>1021</v>
       </c>
       <c r="D359" t="s">
-        <v>1014</v>
+        <v>1022</v>
       </c>
       <c r="E359" t="s">
         <v>1</v>
@@ -10140,13 +10170,16 @@
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
-        <v>1015</v>
+        <v>1023</v>
       </c>
       <c r="B360">
         <v>2020</v>
       </c>
       <c r="C360" t="s">
-        <v>1016</v>
+        <v>1024</v>
+      </c>
+      <c r="D360" t="s">
+        <v>1025</v>
       </c>
       <c r="E360" t="s">
         <v>1</v>
@@ -10154,16 +10187,16 @@
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
-        <v>1017</v>
+        <v>1026</v>
       </c>
       <c r="B361">
         <v>2021</v>
       </c>
       <c r="C361" t="s">
-        <v>1018</v>
+        <v>1027</v>
       </c>
       <c r="D361" t="s">
-        <v>1019</v>
+        <v>1028</v>
       </c>
       <c r="E361" t="s">
         <v>1</v>
@@ -10171,16 +10204,16 @@
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
-        <v>1020</v>
+        <v>1029</v>
       </c>
       <c r="B362">
         <v>2021</v>
       </c>
       <c r="C362" t="s">
-        <v>1021</v>
+        <v>1030</v>
       </c>
       <c r="D362" t="s">
-        <v>1022</v>
+        <v>1031</v>
       </c>
       <c r="E362" t="s">
         <v>1</v>
@@ -10188,16 +10221,16 @@
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
-        <v>1023</v>
+        <v>1032</v>
       </c>
       <c r="B363">
         <v>2020</v>
       </c>
       <c r="C363" t="s">
-        <v>1024</v>
+        <v>1033</v>
       </c>
       <c r="D363" t="s">
-        <v>1025</v>
+        <v>1034</v>
       </c>
       <c r="E363" t="s">
         <v>1</v>
@@ -10205,16 +10238,16 @@
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
-        <v>1026</v>
+        <v>1035</v>
       </c>
       <c r="B364">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C364" t="s">
-        <v>1027</v>
+        <v>1036</v>
       </c>
       <c r="D364" t="s">
-        <v>1028</v>
+        <v>1037</v>
       </c>
       <c r="E364" t="s">
         <v>1</v>
@@ -10222,16 +10255,16 @@
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
-        <v>1029</v>
+        <v>1038</v>
       </c>
       <c r="B365">
         <v>2021</v>
       </c>
       <c r="C365" t="s">
-        <v>1030</v>
+        <v>1039</v>
       </c>
       <c r="D365" t="s">
-        <v>1031</v>
+        <v>1040</v>
       </c>
       <c r="E365" t="s">
         <v>1</v>
@@ -10239,16 +10272,16 @@
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
-        <v>1032</v>
+        <v>1041</v>
       </c>
       <c r="B366">
         <v>2021</v>
       </c>
       <c r="C366" t="s">
-        <v>1033</v>
+        <v>1042</v>
       </c>
       <c r="D366" t="s">
-        <v>1034</v>
+        <v>1043</v>
       </c>
       <c r="E366" t="s">
         <v>1</v>
@@ -10256,16 +10289,13 @@
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
-        <v>1035</v>
+        <v>1044</v>
       </c>
       <c r="B367">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C367" t="s">
-        <v>1036</v>
-      </c>
-      <c r="D367" t="s">
-        <v>1037</v>
+        <v>1045</v>
       </c>
       <c r="E367" t="s">
         <v>1</v>
@@ -10273,16 +10303,16 @@
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
-        <v>1038</v>
+        <v>1046</v>
       </c>
       <c r="B368">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C368" t="s">
-        <v>1039</v>
+        <v>1047</v>
       </c>
       <c r="D368" t="s">
-        <v>1040</v>
+        <v>1048</v>
       </c>
       <c r="E368" t="s">
         <v>1</v>
@@ -10290,16 +10320,16 @@
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
-        <v>1041</v>
+        <v>1049</v>
       </c>
       <c r="B369">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C369" t="s">
-        <v>1042</v>
+        <v>1050</v>
       </c>
       <c r="D369" t="s">
-        <v>1043</v>
+        <v>1051</v>
       </c>
       <c r="E369" t="s">
         <v>1</v>
@@ -10307,16 +10337,16 @@
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
-        <v>1044</v>
+        <v>1052</v>
       </c>
       <c r="B370">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C370" t="s">
-        <v>1045</v>
+        <v>1053</v>
       </c>
       <c r="D370" t="s">
-        <v>1046</v>
+        <v>1054</v>
       </c>
       <c r="E370" t="s">
         <v>1</v>
@@ -10324,13 +10354,16 @@
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
-        <v>1047</v>
+        <v>1055</v>
       </c>
       <c r="B371">
         <v>2021</v>
       </c>
       <c r="C371" t="s">
-        <v>1048</v>
+        <v>1056</v>
+      </c>
+      <c r="D371" t="s">
+        <v>1057</v>
       </c>
       <c r="E371" t="s">
         <v>1</v>
@@ -10338,16 +10371,16 @@
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
-        <v>1049</v>
+        <v>1058</v>
       </c>
       <c r="B372">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C372" t="s">
-        <v>1050</v>
+        <v>1059</v>
       </c>
       <c r="D372" t="s">
-        <v>1051</v>
+        <v>1060</v>
       </c>
       <c r="E372" t="s">
         <v>1</v>
@@ -10355,16 +10388,16 @@
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
-        <v>1052</v>
+        <v>1061</v>
       </c>
       <c r="B373">
         <v>2020</v>
       </c>
       <c r="C373" t="s">
-        <v>1053</v>
+        <v>1062</v>
       </c>
       <c r="D373" t="s">
-        <v>1054</v>
+        <v>1063</v>
       </c>
       <c r="E373" t="s">
         <v>1</v>
@@ -10372,16 +10405,16 @@
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
-        <v>1055</v>
+        <v>1064</v>
       </c>
       <c r="B374">
         <v>2020</v>
       </c>
       <c r="C374" t="s">
-        <v>1056</v>
+        <v>1065</v>
       </c>
       <c r="D374" t="s">
-        <v>1057</v>
+        <v>1066</v>
       </c>
       <c r="E374" t="s">
         <v>1</v>
@@ -10389,16 +10422,16 @@
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
-        <v>1058</v>
+        <v>1067</v>
       </c>
       <c r="B375">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C375" t="s">
-        <v>1059</v>
+        <v>1068</v>
       </c>
       <c r="D375" t="s">
-        <v>1060</v>
+        <v>1069</v>
       </c>
       <c r="E375" t="s">
         <v>1</v>
@@ -10406,16 +10439,13 @@
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
-        <v>1061</v>
+        <v>1070</v>
       </c>
       <c r="B376">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C376" t="s">
-        <v>1062</v>
-      </c>
-      <c r="D376" t="s">
-        <v>1063</v>
+        <v>1071</v>
       </c>
       <c r="E376" t="s">
         <v>1</v>
@@ -10423,16 +10453,16 @@
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
-        <v>1064</v>
+        <v>1072</v>
       </c>
       <c r="B377">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C377" t="s">
-        <v>1065</v>
+        <v>1073</v>
       </c>
       <c r="D377" t="s">
-        <v>1066</v>
+        <v>1074</v>
       </c>
       <c r="E377" t="s">
         <v>1</v>
@@ -10440,16 +10470,16 @@
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
-        <v>1067</v>
+        <v>1075</v>
       </c>
       <c r="B378">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C378" t="s">
-        <v>1068</v>
+        <v>1076</v>
       </c>
       <c r="D378" t="s">
-        <v>1069</v>
+        <v>1077</v>
       </c>
       <c r="E378" t="s">
         <v>1</v>
@@ -10457,16 +10487,16 @@
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
-        <v>1070</v>
+        <v>1078</v>
       </c>
       <c r="B379">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C379" t="s">
-        <v>1071</v>
+        <v>1079</v>
       </c>
       <c r="D379" t="s">
-        <v>1072</v>
+        <v>1080</v>
       </c>
       <c r="E379" t="s">
         <v>1</v>
@@ -10474,13 +10504,16 @@
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
-        <v>1073</v>
+        <v>1081</v>
       </c>
       <c r="B380">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C380" t="s">
-        <v>1074</v>
+        <v>1082</v>
+      </c>
+      <c r="D380" t="s">
+        <v>1083</v>
       </c>
       <c r="E380" t="s">
         <v>1</v>
@@ -10488,16 +10521,16 @@
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
-        <v>1075</v>
+        <v>1084</v>
       </c>
       <c r="B381">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C381" t="s">
-        <v>1076</v>
+        <v>1085</v>
       </c>
       <c r="D381" t="s">
-        <v>1077</v>
+        <v>1086</v>
       </c>
       <c r="E381" t="s">
         <v>1</v>
@@ -10505,16 +10538,16 @@
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
-        <v>1078</v>
+        <v>1087</v>
       </c>
       <c r="B382">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C382" t="s">
-        <v>1079</v>
+        <v>1088</v>
       </c>
       <c r="D382" t="s">
-        <v>1080</v>
+        <v>1089</v>
       </c>
       <c r="E382" t="s">
         <v>1</v>
@@ -10522,16 +10555,16 @@
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
-        <v>1081</v>
+        <v>1090</v>
       </c>
       <c r="B383">
         <v>2021</v>
       </c>
       <c r="C383" t="s">
-        <v>1082</v>
+        <v>1091</v>
       </c>
       <c r="D383" t="s">
-        <v>1083</v>
+        <v>1092</v>
       </c>
       <c r="E383" t="s">
         <v>1</v>
@@ -10539,16 +10572,16 @@
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
-        <v>1084</v>
+        <v>1093</v>
       </c>
       <c r="B384">
         <v>2021</v>
       </c>
       <c r="C384" t="s">
-        <v>1085</v>
+        <v>1094</v>
       </c>
       <c r="D384" t="s">
-        <v>1086</v>
+        <v>1095</v>
       </c>
       <c r="E384" t="s">
         <v>1</v>
@@ -10556,16 +10589,16 @@
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
-        <v>1087</v>
+        <v>1096</v>
       </c>
       <c r="B385">
         <v>2020</v>
       </c>
       <c r="C385" t="s">
-        <v>1088</v>
+        <v>1097</v>
       </c>
       <c r="D385" t="s">
-        <v>1089</v>
+        <v>1098</v>
       </c>
       <c r="E385" t="s">
         <v>1</v>
@@ -10573,16 +10606,16 @@
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
-        <v>1090</v>
+        <v>1099</v>
       </c>
       <c r="B386">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C386" t="s">
-        <v>1091</v>
+        <v>1100</v>
       </c>
       <c r="D386" t="s">
-        <v>1092</v>
+        <v>1101</v>
       </c>
       <c r="E386" t="s">
         <v>1</v>
@@ -10590,16 +10623,16 @@
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A387" t="s">
-        <v>1093</v>
+        <v>1102</v>
       </c>
       <c r="B387">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C387" t="s">
-        <v>1094</v>
+        <v>1103</v>
       </c>
       <c r="D387" t="s">
-        <v>1095</v>
+        <v>1104</v>
       </c>
       <c r="E387" t="s">
         <v>1</v>
@@ -10607,16 +10640,16 @@
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A388" t="s">
-        <v>1096</v>
+        <v>1105</v>
       </c>
       <c r="B388">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C388" t="s">
-        <v>1097</v>
+        <v>1106</v>
       </c>
       <c r="D388" t="s">
-        <v>1098</v>
+        <v>1107</v>
       </c>
       <c r="E388" t="s">
         <v>1</v>
@@ -10624,16 +10657,16 @@
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A389" t="s">
-        <v>1099</v>
+        <v>1108</v>
       </c>
       <c r="B389">
         <v>2020</v>
       </c>
       <c r="C389" t="s">
-        <v>1100</v>
+        <v>1109</v>
       </c>
       <c r="D389" t="s">
-        <v>1101</v>
+        <v>1110</v>
       </c>
       <c r="E389" t="s">
         <v>1</v>
@@ -10641,16 +10674,16 @@
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A390" t="s">
-        <v>1102</v>
+        <v>1111</v>
       </c>
       <c r="B390">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C390" t="s">
-        <v>1103</v>
+        <v>1112</v>
       </c>
       <c r="D390" t="s">
-        <v>1104</v>
+        <v>1113</v>
       </c>
       <c r="E390" t="s">
         <v>1</v>
@@ -10658,16 +10691,16 @@
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A391" t="s">
-        <v>1105</v>
+        <v>1114</v>
       </c>
       <c r="B391">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C391" t="s">
-        <v>1106</v>
+        <v>1115</v>
       </c>
       <c r="D391" t="s">
-        <v>1107</v>
+        <v>1116</v>
       </c>
       <c r="E391" t="s">
         <v>1</v>
@@ -10675,16 +10708,16 @@
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
-        <v>1108</v>
+        <v>1117</v>
       </c>
       <c r="B392">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C392" t="s">
-        <v>1109</v>
+        <v>1118</v>
       </c>
       <c r="D392" t="s">
-        <v>1110</v>
+        <v>1119</v>
       </c>
       <c r="E392" t="s">
         <v>1</v>
@@ -10692,16 +10725,13 @@
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
-        <v>1111</v>
+        <v>1120</v>
       </c>
       <c r="B393">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C393" t="s">
-        <v>1112</v>
-      </c>
-      <c r="D393" t="s">
-        <v>1113</v>
+        <v>1121</v>
       </c>
       <c r="E393" t="s">
         <v>1</v>
@@ -10709,16 +10739,16 @@
     </row>
     <row r="394" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
-        <v>1114</v>
+        <v>1122</v>
       </c>
       <c r="B394">
         <v>2020</v>
       </c>
       <c r="C394" t="s">
-        <v>1115</v>
+        <v>1123</v>
       </c>
       <c r="D394" t="s">
-        <v>1116</v>
+        <v>1124</v>
       </c>
       <c r="E394" t="s">
         <v>1</v>
@@ -10726,16 +10756,16 @@
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A395" t="s">
-        <v>1117</v>
+        <v>1125</v>
       </c>
       <c r="B395">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C395" t="s">
-        <v>1118</v>
+        <v>1126</v>
       </c>
       <c r="D395" t="s">
-        <v>1119</v>
+        <v>1127</v>
       </c>
       <c r="E395" t="s">
         <v>1</v>
@@ -10743,16 +10773,13 @@
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
-        <v>1120</v>
+        <v>1128</v>
       </c>
       <c r="B396">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C396" t="s">
-        <v>1121</v>
-      </c>
-      <c r="D396" t="s">
-        <v>1122</v>
+        <v>1129</v>
       </c>
       <c r="E396" t="s">
         <v>1</v>
@@ -10760,13 +10787,16 @@
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
-        <v>1123</v>
+        <v>1130</v>
       </c>
       <c r="B397">
         <v>2021</v>
       </c>
       <c r="C397" t="s">
-        <v>1124</v>
+        <v>1131</v>
+      </c>
+      <c r="D397" t="s">
+        <v>1132</v>
       </c>
       <c r="E397" t="s">
         <v>1</v>
@@ -10774,16 +10804,16 @@
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
-        <v>1125</v>
+        <v>1133</v>
       </c>
       <c r="B398">
         <v>2020</v>
       </c>
       <c r="C398" t="s">
-        <v>1126</v>
+        <v>1134</v>
       </c>
       <c r="D398" t="s">
-        <v>1127</v>
+        <v>1135</v>
       </c>
       <c r="E398" t="s">
         <v>1</v>
@@ -10791,16 +10821,16 @@
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
-        <v>1128</v>
+        <v>1136</v>
       </c>
       <c r="B399">
         <v>2020</v>
       </c>
       <c r="C399" t="s">
-        <v>1129</v>
+        <v>1137</v>
       </c>
       <c r="D399" t="s">
-        <v>1130</v>
+        <v>1138</v>
       </c>
       <c r="E399" t="s">
         <v>1</v>
@@ -10808,13 +10838,16 @@
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
-        <v>1131</v>
+        <v>1139</v>
       </c>
       <c r="B400">
         <v>2020</v>
       </c>
       <c r="C400" t="s">
-        <v>1132</v>
+        <v>1140</v>
+      </c>
+      <c r="D400" t="s">
+        <v>1141</v>
       </c>
       <c r="E400" t="s">
         <v>1</v>
@@ -10822,16 +10855,16 @@
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
-        <v>1133</v>
+        <v>1142</v>
       </c>
       <c r="B401">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C401" t="s">
-        <v>1134</v>
+        <v>1143</v>
       </c>
       <c r="D401" t="s">
-        <v>1135</v>
+        <v>1144</v>
       </c>
       <c r="E401" t="s">
         <v>1</v>
@@ -10839,16 +10872,16 @@
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
-        <v>1136</v>
+        <v>1145</v>
       </c>
       <c r="B402">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C402" t="s">
-        <v>1137</v>
+        <v>1146</v>
       </c>
       <c r="D402" t="s">
-        <v>1138</v>
+        <v>1147</v>
       </c>
       <c r="E402" t="s">
         <v>1</v>
@@ -10856,16 +10889,16 @@
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
-        <v>1139</v>
+        <v>1148</v>
       </c>
       <c r="B403">
         <v>2020</v>
       </c>
       <c r="C403" t="s">
-        <v>1140</v>
+        <v>1149</v>
       </c>
       <c r="D403" t="s">
-        <v>1141</v>
+        <v>1150</v>
       </c>
       <c r="E403" t="s">
         <v>1</v>
@@ -10873,16 +10906,16 @@
     </row>
     <row r="404" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
-        <v>1142</v>
+        <v>1151</v>
       </c>
       <c r="B404">
         <v>2020</v>
       </c>
       <c r="C404" t="s">
-        <v>1143</v>
+        <v>1152</v>
       </c>
       <c r="D404" t="s">
-        <v>1144</v>
+        <v>1153</v>
       </c>
       <c r="E404" t="s">
         <v>1</v>
@@ -10890,16 +10923,16 @@
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
-        <v>1145</v>
+        <v>1154</v>
       </c>
       <c r="B405">
         <v>2020</v>
       </c>
       <c r="C405" t="s">
-        <v>1146</v>
+        <v>1155</v>
       </c>
       <c r="D405" t="s">
-        <v>1147</v>
+        <v>1156</v>
       </c>
       <c r="E405" t="s">
         <v>1</v>
@@ -10907,16 +10940,16 @@
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
-        <v>1148</v>
+        <v>1157</v>
       </c>
       <c r="B406">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C406" t="s">
-        <v>1149</v>
+        <v>1158</v>
       </c>
       <c r="D406" t="s">
-        <v>1150</v>
+        <v>1159</v>
       </c>
       <c r="E406" t="s">
         <v>1</v>
@@ -10924,16 +10957,16 @@
     </row>
     <row r="407" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
-        <v>1151</v>
+        <v>1160</v>
       </c>
       <c r="B407">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C407" t="s">
-        <v>1152</v>
+        <v>1161</v>
       </c>
       <c r="D407" t="s">
-        <v>1153</v>
+        <v>1162</v>
       </c>
       <c r="E407" t="s">
         <v>1</v>
@@ -10941,16 +10974,16 @@
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
-        <v>1154</v>
+        <v>1163</v>
       </c>
       <c r="B408">
         <v>2020</v>
       </c>
       <c r="C408" t="s">
-        <v>1155</v>
+        <v>1164</v>
       </c>
       <c r="D408" t="s">
-        <v>1156</v>
+        <v>1165</v>
       </c>
       <c r="E408" t="s">
         <v>1</v>
@@ -10958,16 +10991,16 @@
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
-        <v>1157</v>
+        <v>1166</v>
       </c>
       <c r="B409">
         <v>2020</v>
       </c>
       <c r="C409" t="s">
-        <v>1158</v>
+        <v>1167</v>
       </c>
       <c r="D409" t="s">
-        <v>1159</v>
+        <v>1168</v>
       </c>
       <c r="E409" t="s">
         <v>1</v>
@@ -10975,16 +11008,13 @@
     </row>
     <row r="410" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
-        <v>1160</v>
+        <v>1169</v>
       </c>
       <c r="B410">
         <v>2020</v>
       </c>
       <c r="C410" t="s">
-        <v>1161</v>
-      </c>
-      <c r="D410" t="s">
-        <v>1162</v>
+        <v>1170</v>
       </c>
       <c r="E410" t="s">
         <v>1</v>
@@ -10992,16 +11022,16 @@
     </row>
     <row r="411" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
-        <v>1163</v>
+        <v>1171</v>
       </c>
       <c r="B411">
         <v>2021</v>
       </c>
       <c r="C411" t="s">
-        <v>1164</v>
+        <v>1172</v>
       </c>
       <c r="D411" t="s">
-        <v>1165</v>
+        <v>1173</v>
       </c>
       <c r="E411" t="s">
         <v>1</v>
@@ -11009,16 +11039,16 @@
     </row>
     <row r="412" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
-        <v>1166</v>
+        <v>1174</v>
       </c>
       <c r="B412">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C412" t="s">
-        <v>1167</v>
+        <v>1175</v>
       </c>
       <c r="D412" t="s">
-        <v>1168</v>
+        <v>1176</v>
       </c>
       <c r="E412" t="s">
         <v>1</v>
@@ -11026,16 +11056,16 @@
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
-        <v>1169</v>
+        <v>1177</v>
       </c>
       <c r="B413">
         <v>2020</v>
       </c>
       <c r="C413" t="s">
-        <v>1170</v>
+        <v>1178</v>
       </c>
       <c r="D413" t="s">
-        <v>1171</v>
+        <v>1179</v>
       </c>
       <c r="E413" t="s">
         <v>1</v>
@@ -11043,13 +11073,16 @@
     </row>
     <row r="414" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
-        <v>1172</v>
+        <v>1180</v>
       </c>
       <c r="B414">
         <v>2020</v>
       </c>
       <c r="C414" t="s">
-        <v>1173</v>
+        <v>1181</v>
+      </c>
+      <c r="D414" t="s">
+        <v>1182</v>
       </c>
       <c r="E414" t="s">
         <v>1</v>
@@ -11057,16 +11090,16 @@
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
-        <v>1174</v>
+        <v>1183</v>
       </c>
       <c r="B415">
         <v>2021</v>
       </c>
       <c r="C415" t="s">
-        <v>1175</v>
+        <v>1184</v>
       </c>
       <c r="D415" t="s">
-        <v>1176</v>
+        <v>1185</v>
       </c>
       <c r="E415" t="s">
         <v>1</v>
@@ -11074,16 +11107,16 @@
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
-        <v>1177</v>
+        <v>1186</v>
       </c>
       <c r="B416">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C416" t="s">
-        <v>1178</v>
+        <v>1187</v>
       </c>
       <c r="D416" t="s">
-        <v>1179</v>
+        <v>1188</v>
       </c>
       <c r="E416" t="s">
         <v>1</v>
@@ -11091,16 +11124,16 @@
     </row>
     <row r="417" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
-        <v>1180</v>
+        <v>1189</v>
       </c>
       <c r="B417">
         <v>2020</v>
       </c>
       <c r="C417" t="s">
-        <v>1181</v>
+        <v>1190</v>
       </c>
       <c r="D417" t="s">
-        <v>1182</v>
+        <v>1191</v>
       </c>
       <c r="E417" t="s">
         <v>1</v>
@@ -11108,16 +11141,16 @@
     </row>
     <row r="418" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A418" t="s">
-        <v>1183</v>
+        <v>1192</v>
       </c>
       <c r="B418">
         <v>2020</v>
       </c>
       <c r="C418" t="s">
-        <v>1184</v>
+        <v>1193</v>
       </c>
       <c r="D418" t="s">
-        <v>1185</v>
+        <v>1194</v>
       </c>
       <c r="E418" t="s">
         <v>1</v>
@@ -11125,16 +11158,16 @@
     </row>
     <row r="419" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A419" t="s">
-        <v>1186</v>
+        <v>1195</v>
       </c>
       <c r="B419">
         <v>2021</v>
       </c>
       <c r="C419" t="s">
-        <v>1187</v>
+        <v>1196</v>
       </c>
       <c r="D419" t="s">
-        <v>1188</v>
+        <v>1197</v>
       </c>
       <c r="E419" t="s">
         <v>1</v>
@@ -11142,16 +11175,16 @@
     </row>
     <row r="420" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A420" t="s">
-        <v>1189</v>
+        <v>1198</v>
       </c>
       <c r="B420">
         <v>2020</v>
       </c>
       <c r="C420" t="s">
-        <v>1190</v>
+        <v>1199</v>
       </c>
       <c r="D420" t="s">
-        <v>1191</v>
+        <v>1200</v>
       </c>
       <c r="E420" t="s">
         <v>1</v>
@@ -11159,16 +11192,16 @@
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A421" t="s">
-        <v>1192</v>
+        <v>1201</v>
       </c>
       <c r="B421">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C421" t="s">
-        <v>1193</v>
+        <v>1202</v>
       </c>
       <c r="D421" t="s">
-        <v>1194</v>
+        <v>1203</v>
       </c>
       <c r="E421" t="s">
         <v>1</v>
@@ -11176,16 +11209,16 @@
     </row>
     <row r="422" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
-        <v>1195</v>
+        <v>1204</v>
       </c>
       <c r="B422">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C422" t="s">
-        <v>1196</v>
+        <v>1205</v>
       </c>
       <c r="D422" t="s">
-        <v>1197</v>
+        <v>1206</v>
       </c>
       <c r="E422" t="s">
         <v>1</v>
@@ -11193,16 +11226,16 @@
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
-        <v>1198</v>
+        <v>1207</v>
       </c>
       <c r="B423">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C423" t="s">
-        <v>1199</v>
+        <v>1208</v>
       </c>
       <c r="D423" t="s">
-        <v>1200</v>
+        <v>1209</v>
       </c>
       <c r="E423" t="s">
         <v>1</v>
@@ -11210,16 +11243,16 @@
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A424" t="s">
-        <v>1201</v>
+        <v>1210</v>
       </c>
       <c r="B424">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C424" t="s">
-        <v>1202</v>
+        <v>1211</v>
       </c>
       <c r="D424" t="s">
-        <v>1203</v>
+        <v>1212</v>
       </c>
       <c r="E424" t="s">
         <v>1</v>
@@ -11227,16 +11260,13 @@
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
-        <v>1204</v>
+        <v>1213</v>
       </c>
       <c r="B425">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C425" t="s">
-        <v>1205</v>
-      </c>
-      <c r="D425" t="s">
-        <v>1206</v>
+        <v>1214</v>
       </c>
       <c r="E425" t="s">
         <v>1</v>
@@ -11244,16 +11274,16 @@
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A426" t="s">
-        <v>1207</v>
+        <v>1215</v>
       </c>
       <c r="B426">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C426" t="s">
-        <v>1208</v>
+        <v>1216</v>
       </c>
       <c r="D426" t="s">
-        <v>1209</v>
+        <v>1217</v>
       </c>
       <c r="E426" t="s">
         <v>1</v>
@@ -11261,16 +11291,16 @@
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
-        <v>1210</v>
+        <v>1218</v>
       </c>
       <c r="B427">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C427" t="s">
-        <v>1211</v>
+        <v>1219</v>
       </c>
       <c r="D427" t="s">
-        <v>1212</v>
+        <v>1220</v>
       </c>
       <c r="E427" t="s">
         <v>1</v>
@@ -11278,16 +11308,16 @@
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
-        <v>1213</v>
+        <v>1221</v>
       </c>
       <c r="B428">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C428" t="s">
-        <v>1214</v>
+        <v>1222</v>
       </c>
       <c r="D428" t="s">
-        <v>1215</v>
+        <v>1223</v>
       </c>
       <c r="E428" t="s">
         <v>1</v>
@@ -11295,13 +11325,13 @@
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A429" t="s">
-        <v>1216</v>
+        <v>1224</v>
       </c>
       <c r="B429">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C429" t="s">
-        <v>1217</v>
+        <v>1225</v>
       </c>
       <c r="E429" t="s">
         <v>1</v>
@@ -11309,16 +11339,16 @@
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A430" t="s">
-        <v>1218</v>
+        <v>1226</v>
       </c>
       <c r="B430">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C430" t="s">
-        <v>1219</v>
+        <v>1227</v>
       </c>
       <c r="D430" t="s">
-        <v>1220</v>
+        <v>1228</v>
       </c>
       <c r="E430" t="s">
         <v>1</v>
@@ -11326,16 +11356,16 @@
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A431" t="s">
-        <v>1221</v>
+        <v>1229</v>
       </c>
       <c r="B431">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C431" t="s">
-        <v>1222</v>
+        <v>1230</v>
       </c>
       <c r="D431" t="s">
-        <v>1223</v>
+        <v>1231</v>
       </c>
       <c r="E431" t="s">
         <v>1</v>
@@ -11343,16 +11373,16 @@
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A432" t="s">
-        <v>1224</v>
+        <v>1232</v>
       </c>
       <c r="B432">
         <v>2020</v>
       </c>
       <c r="C432" t="s">
-        <v>1225</v>
+        <v>1233</v>
       </c>
       <c r="D432" t="s">
-        <v>1226</v>
+        <v>1234</v>
       </c>
       <c r="E432" t="s">
         <v>1</v>
@@ -11360,13 +11390,16 @@
     </row>
     <row r="433" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A433" t="s">
-        <v>1227</v>
+        <v>1235</v>
       </c>
       <c r="B433">
         <v>2021</v>
       </c>
       <c r="C433" t="s">
-        <v>1228</v>
+        <v>1236</v>
+      </c>
+      <c r="D433" t="s">
+        <v>1237</v>
       </c>
       <c r="E433" t="s">
         <v>1</v>
@@ -11374,16 +11407,16 @@
     </row>
     <row r="434" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A434" t="s">
-        <v>1229</v>
+        <v>1238</v>
       </c>
       <c r="B434">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C434" t="s">
-        <v>1230</v>
+        <v>1239</v>
       </c>
       <c r="D434" t="s">
-        <v>1231</v>
+        <v>1240</v>
       </c>
       <c r="E434" t="s">
         <v>1</v>
@@ -11391,16 +11424,16 @@
     </row>
     <row r="435" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A435" t="s">
-        <v>1232</v>
+        <v>1241</v>
       </c>
       <c r="B435">
         <v>2020</v>
       </c>
       <c r="C435" t="s">
-        <v>1233</v>
+        <v>1242</v>
       </c>
       <c r="D435" t="s">
-        <v>1234</v>
+        <v>1243</v>
       </c>
       <c r="E435" t="s">
         <v>1</v>
@@ -11408,16 +11441,16 @@
     </row>
     <row r="436" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A436" t="s">
-        <v>1235</v>
+        <v>1244</v>
       </c>
       <c r="B436">
         <v>2020</v>
       </c>
       <c r="C436" t="s">
-        <v>1236</v>
+        <v>1245</v>
       </c>
       <c r="D436" t="s">
-        <v>1237</v>
+        <v>1246</v>
       </c>
       <c r="E436" t="s">
         <v>1</v>
@@ -11425,16 +11458,16 @@
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A437" t="s">
-        <v>1238</v>
+        <v>1247</v>
       </c>
       <c r="B437">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C437" t="s">
-        <v>1239</v>
+        <v>1248</v>
       </c>
       <c r="D437" t="s">
-        <v>1240</v>
+        <v>1249</v>
       </c>
       <c r="E437" t="s">
         <v>1</v>
@@ -11442,16 +11475,16 @@
     </row>
     <row r="438" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A438" t="s">
-        <v>1241</v>
+        <v>1250</v>
       </c>
       <c r="B438">
         <v>2020</v>
       </c>
       <c r="C438" t="s">
-        <v>1242</v>
+        <v>1251</v>
       </c>
       <c r="D438" t="s">
-        <v>1243</v>
+        <v>1252</v>
       </c>
       <c r="E438" t="s">
         <v>1</v>
@@ -11459,16 +11492,16 @@
     </row>
     <row r="439" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A439" t="s">
-        <v>1244</v>
+        <v>1253</v>
       </c>
       <c r="B439">
         <v>2020</v>
       </c>
       <c r="C439" t="s">
-        <v>1245</v>
+        <v>1254</v>
       </c>
       <c r="D439" t="s">
-        <v>1246</v>
+        <v>1255</v>
       </c>
       <c r="E439" t="s">
         <v>1</v>
@@ -11476,86 +11509,18 @@
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A440" t="s">
-        <v>1247</v>
+        <v>1256</v>
       </c>
       <c r="B440">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C440" t="s">
-        <v>1248</v>
+        <v>1257</v>
       </c>
       <c r="D440" t="s">
-        <v>1249</v>
+        <v>1258</v>
       </c>
       <c r="E440" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A441" t="s">
-        <v>1250</v>
-      </c>
-      <c r="B441">
-        <v>2020</v>
-      </c>
-      <c r="C441" t="s">
-        <v>1251</v>
-      </c>
-      <c r="D441" t="s">
-        <v>1252</v>
-      </c>
-      <c r="E441" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A442" t="s">
-        <v>1253</v>
-      </c>
-      <c r="B442">
-        <v>2020</v>
-      </c>
-      <c r="C442" t="s">
-        <v>1254</v>
-      </c>
-      <c r="D442" t="s">
-        <v>1255</v>
-      </c>
-      <c r="E442" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A443" t="s">
-        <v>1256</v>
-      </c>
-      <c r="B443">
-        <v>2020</v>
-      </c>
-      <c r="C443" t="s">
-        <v>1257</v>
-      </c>
-      <c r="D443" t="s">
-        <v>1258</v>
-      </c>
-      <c r="E443" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A444" t="s">
-        <v>1259</v>
-      </c>
-      <c r="B444">
-        <v>2021</v>
-      </c>
-      <c r="C444" t="s">
-        <v>1260</v>
-      </c>
-      <c r="D444" t="s">
-        <v>1261</v>
-      </c>
-      <c r="E444" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>